<commit_message>
setup feature files, page classes and step definitions
</commit_message>
<xml_diff>
--- a/src/test/java/testData/TestData_Buildxact.xlsx
+++ b/src/test/java/testData/TestData_Buildxact.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shalini\Automation projects\src\test\java\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shalini\Documents\IntelliJ Projects\BuildxactApplicationTesting\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -440,7 +440,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +473,10 @@
         <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -487,20 +487,20 @@
         <v>9</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="D3" r:id="rId5"/>
-    <hyperlink ref="D2" r:id="rId6"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="D2" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
+    <hyperlink ref="D3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -511,7 +511,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>